<commit_message>
Update Mercy Pricing Model
Do this to reflect an existing collaborative discount (discount is based
on the the basic collaborative services quarterly only, $3,525 a year)
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/1111MHS - Mercy Health/Pricing_Model_1111MHS_2018-02-22.xlsx
+++ b/0273NYP - New York Premier/1111MHS - Mercy Health/Pricing_Model_1111MHS_2018-02-22.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="0" windowWidth="13680" windowHeight="13890" activeTab="3"/>
+    <workbookView xWindow="1395" yWindow="0" windowWidth="13680" windowHeight="13890"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="ACOInsight1">Inputs!$D$18:$D$19</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">Outputs_Internal!$B$1:$M$55</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">Outputs_Internal!$B$1:$M$56</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="105">
   <si>
     <t>One-Time Fees:</t>
   </si>
@@ -346,6 +346,9 @@
   <si>
     <t>MI Royalties</t>
   </si>
+  <si>
+    <t>Existing Collaborative Discount</t>
+  </si>
 </sst>
 </file>
 
@@ -582,7 +585,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -725,6 +728,9 @@
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="9" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1021,11 +1027,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L21"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,13 +1321,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:U42"/>
+  <dimension ref="B2:U43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2019,44 +2025,53 @@
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
     </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B29" s="6" t="s">
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>104</v>
+      </c>
+      <c r="D28" s="1">
+        <f>Calcs!D92</f>
+        <v>-3525</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B30" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="7">
-        <f>SUM(D7:D17, D20:D23, D26:D27)</f>
-        <v>57600</v>
-      </c>
-      <c r="E29" s="7">
-        <f t="shared" ref="E29:H29" si="0">SUM(E7:E17, E20:E23, E26:E27)</f>
-        <v>0</v>
-      </c>
-      <c r="F29" s="7">
+      <c r="D30" s="7">
+        <f>SUM(D7:D17, D20:D23, D26:D28)</f>
+        <v>54075</v>
+      </c>
+      <c r="E30" s="7">
+        <f t="shared" ref="E30:H30" si="0">SUM(E7:E17, E20:E23, E26:E27)</f>
+        <v>0</v>
+      </c>
+      <c r="F30" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G30" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H29" s="7">
+      <c r="H30" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="M29" s="1"/>
-      <c r="S29" s="1"/>
-      <c r="T29" s="1"/>
-      <c r="U29" s="1"/>
-    </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
@@ -2066,9 +2081,6 @@
       <c r="U30" s="1"/>
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B31" s="6" t="s">
-        <v>98</v>
-      </c>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
@@ -2078,99 +2090,116 @@
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
       <c r="M31" s="1"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
     </row>
     <row r="32" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C32" s="68">
+      <c r="B32" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="M32" s="1"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+    </row>
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C33" s="68">
         <f>INDEX(Outputs_Timeline!$D$3:$D$94,MATCH(Inputs!$C$1,Outputs_Timeline!$B$3:$B$94,0),1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B34" s="6" t="s">
+    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B35" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="D34" s="7">
-        <f>(D29/12*Inputs!$C$2+D4)*$C$32</f>
-        <v>172800</v>
-      </c>
-      <c r="E34" s="7">
-        <f>(E29/12*Inputs!$C$2+E4)*$C$32</f>
-        <v>0</v>
-      </c>
-      <c r="F34" s="7">
-        <f>(F29/12*Inputs!$C$2+F4)*$C$32</f>
-        <v>0</v>
-      </c>
-      <c r="G34" s="7">
-        <f>(G29/12*Inputs!$C$2+G4)*$C$32</f>
-        <v>0</v>
-      </c>
-      <c r="H34" s="7">
-        <f>(H29/12*Inputs!$C$2+H4)*$C$32</f>
-        <v>0</v>
-      </c>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="7"/>
-      <c r="M34" s="1"/>
-      <c r="S34" s="1"/>
-      <c r="T34" s="1"/>
-      <c r="U34" s="1"/>
-    </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7"/>
-      <c r="M36" s="1"/>
-      <c r="S36" s="8"/>
-      <c r="T36" s="8"/>
-      <c r="U36" s="8"/>
+      <c r="D35" s="7">
+        <f>(D30/12*Inputs!$C$2+D4)*$C$33</f>
+        <v>162225</v>
+      </c>
+      <c r="E35" s="7">
+        <f>(E30/12*Inputs!$C$2+E4)*$C$33</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="7">
+        <f>(F30/12*Inputs!$C$2+F4)*$C$33</f>
+        <v>0</v>
+      </c>
+      <c r="G35" s="7">
+        <f>(G30/12*Inputs!$C$2+G4)*$C$33</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="7">
+        <f>(H30/12*Inputs!$C$2+H4)*$C$33</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="M35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
     </row>
     <row r="37" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B37" s="6" t="s">
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="1"/>
+      <c r="S37" s="8"/>
+      <c r="T37" s="8"/>
+      <c r="U37" s="8"/>
+    </row>
+    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B38" s="6" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C38" s="7">
+    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C39" s="7">
         <f>SUM(Outputs_Timeline!S:S)</f>
-        <v>172800</v>
-      </c>
-    </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C39" s="53">
-        <f>SUM(D34:H34)</f>
-        <v>172800</v>
-      </c>
-      <c r="D39" s="1"/>
-      <c r="G39" s="1"/>
+        <v>162225</v>
+      </c>
     </row>
     <row r="40" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C40" s="53">
+        <f>SUM(D35:H35)</f>
+        <v>162225</v>
+      </c>
       <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
     </row>
     <row r="41" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="D41" s="2"/>
+      <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2182,13 +2211,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:N62"/>
+  <dimension ref="B1:N63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
+      <selection pane="bottomRight" activeCell="Q36" sqref="Q36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2202,8 +2231,7 @@
     <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="3.85546875" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -3639,19 +3667,19 @@
         <v>0</v>
       </c>
       <c r="F48" s="8">
-        <f>IFERROR(SUM(K59:K62)/SUM($K$59:$M$62), 0)</f>
+        <f>IFERROR(SUM(K60:K63)/SUM($K$60:$M$63), 0)</f>
         <v>0.59922896413007043</v>
       </c>
       <c r="G48" s="8">
-        <f>IFERROR(SUM(L59:L62)/SUM($K$59:$M$62), 0)</f>
+        <f>IFERROR(SUM(L60:L63)/SUM($K$60:$M$63), 0)</f>
         <v>0.2550564308861325</v>
       </c>
       <c r="H48" s="8">
-        <f>IFERROR(SUM(M59:M62)/SUM($K$59:$M$62), 0)</f>
+        <f>IFERROR(SUM(M60:M63)/SUM($K$60:$M$63), 0)</f>
         <v>0.1457146049837971</v>
       </c>
       <c r="I48" s="8">
-        <f>IFERROR(SUM(N59:N62)/SUM($K$59:$M$62), 0)</f>
+        <f>IFERROR(SUM(N60:N63)/SUM($K$60:$M$63), 0)</f>
         <v>1.2142883748649757E-2</v>
       </c>
       <c r="K48" s="12">
@@ -3713,290 +3741,328 @@
       </c>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K50" s="9"/>
-      <c r="L50" s="9"/>
-      <c r="M50" s="9"/>
+      <c r="C50" t="s">
+        <v>104</v>
+      </c>
+      <c r="D50" s="1">
+        <f>Outputs_External!D28</f>
+        <v>-3525</v>
+      </c>
+      <c r="F50" s="3">
+        <v>0.58085106382978702</v>
+      </c>
+      <c r="G50" s="3">
+        <f>1-F50</f>
+        <v>0.41914893617021298</v>
+      </c>
+      <c r="H50" s="3">
+        <v>0</v>
+      </c>
+      <c r="I50" s="3">
+        <v>0</v>
+      </c>
+      <c r="K50" s="82">
+        <f>F50*$D$50</f>
+        <v>-2047.4999999999993</v>
+      </c>
+      <c r="L50" s="82">
+        <f t="shared" ref="L50:N50" si="18">G50*$D$50</f>
+        <v>-1477.5000000000007</v>
+      </c>
+      <c r="M50" s="82">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="N50" s="82">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B51" s="6" t="s">
+      <c r="K51" s="9"/>
+      <c r="L51" s="9"/>
+      <c r="M51" s="9"/>
+    </row>
+    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B52" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D51" s="1">
-        <f>SUM(Outputs_External!D29:'Outputs_External'!H29)</f>
-        <v>57600</v>
-      </c>
-      <c r="K51" s="12">
-        <f>SUM(K48:K49, K36:K39, K8:K18,K23:K33,K42:K45)</f>
-        <v>30600</v>
-      </c>
-      <c r="L51" s="12">
-        <f t="shared" ref="L51" si="18">SUM(L48:L49, L36:L39, L8:L18,L23:L33,L42:L45)</f>
-        <v>20760</v>
-      </c>
-      <c r="M51" s="12">
-        <f>SUM(M48:M49, M36:M39, M8:M18,M23:M33,M42:M45)</f>
+      <c r="D52" s="1">
+        <f>SUM(Outputs_External!D30:'Outputs_External'!H30)</f>
+        <v>54075</v>
+      </c>
+      <c r="K52" s="12">
+        <f>SUM(K48:K50, K36:K39, K8:K18,K23:K33,K42:K45)</f>
+        <v>28552.5</v>
+      </c>
+      <c r="L52" s="12">
+        <f t="shared" ref="L52:N52" si="19">SUM(L48:L50, L36:L39, L8:L18,L23:L33,L42:L45)</f>
+        <v>19282.5</v>
+      </c>
+      <c r="M52" s="12">
+        <f t="shared" si="19"/>
         <v>5760</v>
       </c>
-      <c r="N51" s="12">
-        <f>SUM(N48:N49, N36:N39, N8:N18,N23:N33,N42:N45)</f>
+      <c r="N52" s="12">
+        <f t="shared" si="19"/>
         <v>480</v>
       </c>
     </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C52" s="21" t="s">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C53" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="D52" s="23">
-        <f>SUM(K51:N51)</f>
-        <v>57600</v>
-      </c>
-      <c r="K52" s="12"/>
-      <c r="L52" s="12"/>
-      <c r="M52" s="12"/>
-    </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K53" s="9"/>
-      <c r="L53" s="9"/>
-      <c r="M53" s="9"/>
+      <c r="D53" s="23">
+        <f>SUM(K52:N52)</f>
+        <v>54075</v>
+      </c>
+      <c r="K53" s="12"/>
+      <c r="L53" s="12"/>
+      <c r="M53" s="12"/>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B54" s="6" t="s">
+      <c r="K54" s="9"/>
+      <c r="L54" s="9"/>
+      <c r="M54" s="9"/>
+    </row>
+    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B55" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D54" s="1">
+      <c r="D55" s="1">
         <f>SUM(Outputs_Timeline!S:S)</f>
-        <v>172800</v>
-      </c>
-      <c r="K54" s="12">
+        <v>162225</v>
+      </c>
+      <c r="K55" s="12">
         <f>SUM(Outputs_Timeline!T:T)</f>
-        <v>91800</v>
-      </c>
-      <c r="L54" s="12">
+        <v>85657.5</v>
+      </c>
+      <c r="L55" s="12">
         <f>SUM(Outputs_Timeline!U:U)</f>
-        <v>62280</v>
-      </c>
-      <c r="M54" s="12">
+        <v>57847.5</v>
+      </c>
+      <c r="M55" s="12">
         <f>SUM(Outputs_Timeline!V:V)</f>
         <v>17280</v>
       </c>
-      <c r="N54" s="12">
+      <c r="N55" s="12">
         <f>SUM(Outputs_Timeline!W:W)</f>
         <v>1440</v>
       </c>
     </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D55" s="1"/>
-      <c r="K55" s="54">
-        <f>IFERROR(K54/$D$54, 0)</f>
-        <v>0.53125</v>
-      </c>
-      <c r="L55" s="54">
-        <f>IFERROR(L54/$D$54, 0)</f>
-        <v>0.36041666666666666</v>
-      </c>
-      <c r="M55" s="54">
-        <f>IFERROR(M54/$D$54, 0)</f>
-        <v>0.1</v>
-      </c>
-      <c r="N55" s="54">
-        <f>IFERROR(N54/$D$54, 0)</f>
-        <v>8.3333333333333332E-3</v>
-      </c>
-    </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K57" s="9"/>
-      <c r="L57" s="9"/>
-      <c r="M57" s="9"/>
+    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D56" s="1"/>
+      <c r="K56" s="54">
+        <f>IFERROR(K55/$D$55, 0)</f>
+        <v>0.52801664355062417</v>
+      </c>
+      <c r="L56" s="54">
+        <f>IFERROR(L55/$D$55, 0)</f>
+        <v>0.35658807212205268</v>
+      </c>
+      <c r="M56" s="54">
+        <f>IFERROR(M55/$D$55, 0)</f>
+        <v>0.10651872399445216</v>
+      </c>
+      <c r="N56" s="54">
+        <f>IFERROR(N55/$D$55, 0)</f>
+        <v>8.8765603328710124E-3</v>
+      </c>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B58" s="27" t="s">
+      <c r="K58" s="9"/>
+      <c r="L58" s="9"/>
+      <c r="M58" s="9"/>
+    </row>
+    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B59" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="C58" s="21"/>
-      <c r="D58" s="21"/>
-      <c r="E58" s="21"/>
-      <c r="F58" s="21"/>
-      <c r="G58" s="21"/>
-      <c r="H58" s="21"/>
-      <c r="I58" s="21"/>
-      <c r="J58" s="21"/>
-      <c r="K58" s="22"/>
-      <c r="L58" s="22"/>
-      <c r="M58" s="22"/>
-    </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B59" s="27"/>
-      <c r="C59" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D59" s="23">
-        <f>SUM(Calcs!D61:H61)+SUM(Calcs!D67:H67)</f>
-        <v>0</v>
-      </c>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
       <c r="E59" s="21"/>
-      <c r="F59" s="24">
-        <f>F36</f>
-        <v>0.9</v>
-      </c>
-      <c r="G59" s="24">
-        <f>G36</f>
-        <v>0.1</v>
-      </c>
-      <c r="H59" s="24">
-        <f>H36</f>
-        <v>0</v>
-      </c>
-      <c r="I59" s="24">
-        <f>I36</f>
-        <v>0</v>
-      </c>
+      <c r="F59" s="21"/>
+      <c r="G59" s="21"/>
+      <c r="H59" s="21"/>
+      <c r="I59" s="21"/>
       <c r="J59" s="21"/>
-      <c r="K59" s="25">
-        <f t="shared" ref="K59:N62" si="19">F59*$D59</f>
-        <v>0</v>
-      </c>
-      <c r="L59" s="25">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="M59" s="25">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="N59" s="25">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
+      <c r="K59" s="22"/>
+      <c r="L59" s="22"/>
+      <c r="M59" s="22"/>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B60" s="27"/>
       <c r="C60" s="21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D60" s="23">
-        <f>SUM(Calcs!D62:H62)+SUM(Calcs!D68:H68)</f>
-        <v>39600</v>
+        <f>SUM(Calcs!D61:H61)+SUM(Calcs!D67:H67)</f>
+        <v>0</v>
       </c>
       <c r="E60" s="21"/>
       <c r="F60" s="24">
-        <f>IFERROR(SUM(K$37,K$10:K$15,K$43,K$25:K$30)/SUM($K$37:$M$37,$K$10:$M$15,$K$43:$M$43,$K$25:$M$30),0)</f>
-        <v>0.59815950920245398</v>
+        <f>F36</f>
+        <v>0.9</v>
       </c>
       <c r="G60" s="24">
-        <f t="shared" ref="G60" si="20">IFERROR(SUM(L$37,L$10:L$15,L$43,L$25:L$30)/SUM($K$37:$M$37,$K$10:$M$15,$K$43:$M$43,$K$25:$M$30),0)</f>
-        <v>0.254601226993865</v>
+        <f>G36</f>
+        <v>0.1</v>
       </c>
       <c r="H60" s="24">
-        <f>IFERROR(SUM(M$37,M$10:M$15,M$43,M$25:M$30)/SUM($K$37:$N$37,$K$10:$N$15,$K$43:$N$43,$K$25:$N$30),0)</f>
-        <v>0.14545454545454545</v>
+        <f>H36</f>
+        <v>0</v>
       </c>
       <c r="I60" s="24">
-        <f>IFERROR(SUM(N$37,N$10:N$15,N$43,N$25:N$30)/SUM($K$37:$N$37,$K$10:$N$15,$K$43:$N$43,$K$25:$N$30),0)</f>
-        <v>1.2121212121212121E-2</v>
+        <f>I36</f>
+        <v>0</v>
       </c>
       <c r="J60" s="21"/>
       <c r="K60" s="25">
-        <f t="shared" si="19"/>
-        <v>23687.116564417178</v>
+        <f t="shared" ref="K60:N63" si="20">F60*$D60</f>
+        <v>0</v>
       </c>
       <c r="L60" s="25">
-        <f t="shared" si="19"/>
-        <v>10082.208588957054</v>
+        <f t="shared" si="20"/>
+        <v>0</v>
       </c>
       <c r="M60" s="25">
-        <f t="shared" si="19"/>
-        <v>5760</v>
+        <f t="shared" si="20"/>
+        <v>0</v>
       </c>
       <c r="N60" s="25">
-        <f t="shared" si="19"/>
-        <v>480</v>
+        <f t="shared" si="20"/>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B61" s="27"/>
       <c r="C61" s="21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D61" s="23">
-        <f>SUM(Calcs!D63:H63)+SUM(Calcs!D69:H69)</f>
-        <v>0</v>
+        <f>SUM(Calcs!D62:H62)+SUM(Calcs!D68:H68)</f>
+        <v>39600</v>
       </c>
       <c r="E61" s="21"/>
       <c r="F61" s="24">
-        <f>IFERROR(SUM(K38,K16:K18,K44,K31:K33)/SUM($K$38:$M$38,$K$16:$M$18,$K$44:$M$44,$K$31:$M$33),0)</f>
-        <v>0</v>
+        <f>IFERROR(SUM(K$37,K$10:K$15,K$43,K$25:K$30)/SUM($K$37:$M$37,$K$10:$M$15,$K$43:$M$43,$K$25:$M$30),0)</f>
+        <v>0.59815950920245398</v>
       </c>
       <c r="G61" s="24">
-        <f>IFERROR(SUM(L38,L16:L18,L44,L31:L33)/SUM($K$38:$M$38,$K$16:$M$18,$K$44:$M$44,$K$31:$M$33),0)</f>
-        <v>0</v>
+        <f t="shared" ref="G61" si="21">IFERROR(SUM(L$37,L$10:L$15,L$43,L$25:L$30)/SUM($K$37:$M$37,$K$10:$M$15,$K$43:$M$43,$K$25:$M$30),0)</f>
+        <v>0.254601226993865</v>
       </c>
       <c r="H61" s="24">
-        <f>IFERROR(SUM(M38,M16:M18,M44,M31:M33)/SUM($K$38:$N$38,$K$16:$N$18,$K$44:$N$44,$K$31:$N$33),0)</f>
-        <v>0</v>
+        <f>IFERROR(SUM(M$37,M$10:M$15,M$43,M$25:M$30)/SUM($K$37:$N$37,$K$10:$N$15,$K$43:$N$43,$K$25:$N$30),0)</f>
+        <v>0.14545454545454545</v>
       </c>
       <c r="I61" s="24">
-        <f>IFERROR(SUM(N38,N16:N18,N44,N31:N33)/SUM($K$38:$N$38,$K$16:$N$18,$K$44:$N$44,$K$31:$N$33),0)</f>
-        <v>0</v>
+        <f>IFERROR(SUM(N$37,N$10:N$15,N$43,N$25:N$30)/SUM($K$37:$N$37,$K$10:$N$15,$K$43:$N$43,$K$25:$N$30),0)</f>
+        <v>1.2121212121212121E-2</v>
       </c>
       <c r="J61" s="21"/>
       <c r="K61" s="25">
-        <f t="shared" si="19"/>
-        <v>0</v>
+        <f t="shared" si="20"/>
+        <v>23687.116564417178</v>
       </c>
       <c r="L61" s="25">
-        <f t="shared" si="19"/>
-        <v>0</v>
+        <f t="shared" si="20"/>
+        <v>10082.208588957054</v>
       </c>
       <c r="M61" s="25">
-        <f t="shared" si="19"/>
-        <v>0</v>
+        <f t="shared" si="20"/>
+        <v>5760</v>
       </c>
       <c r="N61" s="25">
-        <f t="shared" si="19"/>
-        <v>0</v>
+        <f t="shared" si="20"/>
+        <v>480</v>
       </c>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B62" s="27"/>
       <c r="C62" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D62" s="23">
-        <f>SUM(Calcs!D64:H64)+SUM(Calcs!D70:H70)</f>
+        <f>SUM(Calcs!D63:H63)+SUM(Calcs!D69:H69)</f>
         <v>0</v>
       </c>
       <c r="E62" s="21"/>
       <c r="F62" s="24">
+        <f>IFERROR(SUM(K38,K16:K18,K44,K31:K33)/SUM($K$38:$M$38,$K$16:$M$18,$K$44:$M$44,$K$31:$M$33),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G62" s="24">
+        <f>IFERROR(SUM(L38,L16:L18,L44,L31:L33)/SUM($K$38:$M$38,$K$16:$M$18,$K$44:$M$44,$K$31:$M$33),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H62" s="24">
+        <f>IFERROR(SUM(M38,M16:M18,M44,M31:M33)/SUM($K$38:$N$38,$K$16:$N$18,$K$44:$N$44,$K$31:$N$33),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I62" s="24">
+        <f>IFERROR(SUM(N38,N16:N18,N44,N31:N33)/SUM($K$38:$N$38,$K$16:$N$18,$K$44:$N$44,$K$31:$N$33),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J62" s="21"/>
+      <c r="K62" s="25">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="L62" s="25">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="M62" s="25">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="N62" s="25">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B63" s="27"/>
+      <c r="C63" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D63" s="23">
+        <f>SUM(Calcs!D64:H64)+SUM(Calcs!D70:H70)</f>
+        <v>0</v>
+      </c>
+      <c r="E63" s="21"/>
+      <c r="F63" s="24">
         <f>F39</f>
         <v>0.1</v>
       </c>
-      <c r="G62" s="24">
+      <c r="G63" s="24">
         <f>G39</f>
         <v>0.9</v>
       </c>
-      <c r="H62" s="24">
+      <c r="H63" s="24">
         <f>H39</f>
         <v>0</v>
       </c>
-      <c r="I62" s="24">
+      <c r="I63" s="24">
         <f>I39</f>
         <v>0</v>
       </c>
-      <c r="J62" s="21"/>
-      <c r="K62" s="25">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="L62" s="25">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="M62" s="25">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="N62" s="25">
-        <f t="shared" si="19"/>
+      <c r="J63" s="21"/>
+      <c r="K63" s="25">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="L63" s="25">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="M63" s="25">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="N63" s="25">
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -4010,11 +4076,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P9" sqref="P9:P44"/>
+      <selection pane="bottomRight" activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4152,23 +4218,23 @@
         <v>0</v>
       </c>
       <c r="M3" s="67">
-        <f>$F3*Outputs_Internal!$D$51/12</f>
+        <f>$F3*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N3" s="67">
-        <f>$F3*Outputs_Internal!K$51/12</f>
+        <f>$F3*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O3" s="67">
-        <f>$F3*Outputs_Internal!L$51/12</f>
+        <f>$F3*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P3" s="67">
-        <f>$F3*Outputs_Internal!M$51/12</f>
+        <f>$F3*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q3" s="67">
-        <f>$F3*Outputs_Internal!N$51/12</f>
+        <f>$F3*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S3" s="67"/>
@@ -4210,23 +4276,23 @@
         <v>0</v>
       </c>
       <c r="M4" s="67">
-        <f>$F4*Outputs_Internal!$D$51/12</f>
+        <f>$F4*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N4" s="67">
-        <f>$F4*Outputs_Internal!K$51/12</f>
+        <f>$F4*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O4" s="67">
-        <f>$F4*Outputs_Internal!L$51/12</f>
+        <f>$F4*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P4" s="67">
-        <f>$F4*Outputs_Internal!M$51/12</f>
+        <f>$F4*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q4" s="67">
-        <f>$F4*Outputs_Internal!N$51/12</f>
+        <f>$F4*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
     </row>
@@ -4264,23 +4330,23 @@
         <v>0</v>
       </c>
       <c r="M5" s="67">
-        <f>$F5*Outputs_Internal!$D$51/12</f>
+        <f>$F5*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N5" s="67">
-        <f>$F5*Outputs_Internal!K$51/12</f>
+        <f>$F5*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O5" s="67">
-        <f>$F5*Outputs_Internal!L$51/12</f>
+        <f>$F5*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P5" s="67">
-        <f>$F5*Outputs_Internal!M$51/12</f>
+        <f>$F5*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q5" s="67">
-        <f>$F5*Outputs_Internal!N$51/12</f>
+        <f>$F5*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S5" s="67">
@@ -4338,23 +4404,23 @@
         <v>0</v>
       </c>
       <c r="M6" s="67">
-        <f>$F6*Outputs_Internal!$D$51/12</f>
+        <f>$F6*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N6" s="67">
-        <f>$F6*Outputs_Internal!K$51/12</f>
+        <f>$F6*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O6" s="67">
-        <f>$F6*Outputs_Internal!L$51/12</f>
+        <f>$F6*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P6" s="67">
-        <f>$F6*Outputs_Internal!M$51/12</f>
+        <f>$F6*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q6" s="67">
-        <f>$F6*Outputs_Internal!N$51/12</f>
+        <f>$F6*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S6" s="67">
@@ -4412,23 +4478,23 @@
         <v>0</v>
       </c>
       <c r="M7" s="67">
-        <f>$F7*Outputs_Internal!$D$51/12</f>
+        <f>$F7*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N7" s="67">
-        <f>$F7*Outputs_Internal!K$51/12</f>
+        <f>$F7*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O7" s="67">
-        <f>$F7*Outputs_Internal!L$51/12</f>
+        <f>$F7*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P7" s="67">
-        <f>$F7*Outputs_Internal!M$51/12</f>
+        <f>$F7*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q7" s="67">
-        <f>$F7*Outputs_Internal!N$51/12</f>
+        <f>$F7*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S7" s="67">
@@ -4486,23 +4552,23 @@
         <v>0</v>
       </c>
       <c r="M8" s="67">
-        <f>$F8*Outputs_Internal!$D$51/12</f>
+        <f>$F8*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N8" s="67">
-        <f>$F8*Outputs_Internal!K$51/12</f>
+        <f>$F8*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O8" s="67">
-        <f>$F8*Outputs_Internal!L$51/12</f>
+        <f>$F8*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P8" s="67">
-        <f>$F8*Outputs_Internal!M$51/12</f>
+        <f>$F8*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q8" s="67">
-        <f>$F8*Outputs_Internal!N$51/12</f>
+        <f>$F8*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S8" s="67">
@@ -4560,23 +4626,23 @@
         <v>0</v>
       </c>
       <c r="M9" s="67">
-        <f>$F9*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F9*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N9" s="67">
-        <f>$F9*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F9*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O9" s="67">
-        <f>$F9*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F9*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P9" s="67">
-        <f>$F9*Outputs_Internal!M$51/12</f>
+        <f>$F9*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q9" s="67">
-        <f>$F9*Outputs_Internal!N$51/12</f>
+        <f>$F9*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S9" s="67">
@@ -4634,23 +4700,23 @@
         <v>0</v>
       </c>
       <c r="M10" s="67">
-        <f>$F10*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F10*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N10" s="67">
-        <f>$F10*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F10*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O10" s="67">
-        <f>$F10*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F10*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P10" s="67">
-        <f>$F10*Outputs_Internal!M$51/12</f>
+        <f>$F10*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q10" s="67">
-        <f>$F10*Outputs_Internal!N$51/12</f>
+        <f>$F10*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S10" s="67">
@@ -4708,36 +4774,36 @@
         <v>0</v>
       </c>
       <c r="M11" s="67">
-        <f>$F11*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F11*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N11" s="67">
-        <f>$F11*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F11*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O11" s="67">
-        <f>$F11*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F11*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P11" s="67">
-        <f>$F11*Outputs_Internal!M$51/12</f>
+        <f>$F11*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q11" s="67">
-        <f>$F11*Outputs_Internal!N$51/12</f>
+        <f>$F11*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S11" s="67">
         <f t="shared" si="1"/>
-        <v>14400</v>
+        <v>13518.75</v>
       </c>
       <c r="T11" s="67">
         <f t="shared" si="2"/>
-        <v>7650</v>
+        <v>7138.125</v>
       </c>
       <c r="U11" s="67">
         <f>IF(MOD(MONTH($B11),3)=0,SUM(J9:J11,O9:O11),0)</f>
-        <v>5190</v>
+        <v>4820.625</v>
       </c>
       <c r="V11" s="67">
         <f t="shared" si="4"/>
@@ -4782,23 +4848,23 @@
         <v>0</v>
       </c>
       <c r="M12" s="67">
-        <f>$F12*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F12*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N12" s="67">
-        <f>$F12*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F12*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O12" s="67">
-        <f>$F12*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F12*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P12" s="67">
-        <f>$F12*Outputs_Internal!M$51/12</f>
+        <f>$F12*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q12" s="67">
-        <f>$F12*Outputs_Internal!N$51/12</f>
+        <f>$F12*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S12" s="67">
@@ -4856,23 +4922,23 @@
         <v>0</v>
       </c>
       <c r="M13" s="67">
-        <f>$F13*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F13*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N13" s="67">
-        <f>$F13*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F13*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O13" s="67">
-        <f>$F13*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F13*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P13" s="67">
-        <f>$F13*Outputs_Internal!M$51/12</f>
+        <f>$F13*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q13" s="67">
-        <f>$F13*Outputs_Internal!N$51/12</f>
+        <f>$F13*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S13" s="67">
@@ -4930,36 +4996,36 @@
         <v>0</v>
       </c>
       <c r="M14" s="67">
-        <f>$F14*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F14*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N14" s="67">
-        <f>$F14*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F14*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O14" s="67">
-        <f>$F14*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F14*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P14" s="67">
-        <f>$F14*Outputs_Internal!M$51/12</f>
+        <f>$F14*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q14" s="67">
-        <f>$F14*Outputs_Internal!N$51/12</f>
+        <f>$F14*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S14" s="67">
         <f t="shared" si="1"/>
-        <v>14400</v>
+        <v>13518.75</v>
       </c>
       <c r="T14" s="67">
         <f t="shared" si="2"/>
-        <v>7650</v>
+        <v>7138.125</v>
       </c>
       <c r="U14" s="67">
         <f t="shared" si="3"/>
-        <v>5190</v>
+        <v>4820.625</v>
       </c>
       <c r="V14" s="67">
         <f t="shared" si="4"/>
@@ -5004,23 +5070,23 @@
         <v>0</v>
       </c>
       <c r="M15" s="67">
-        <f>$F15*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F15*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N15" s="67">
-        <f>$F15*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F15*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O15" s="67">
-        <f>$F15*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F15*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P15" s="67">
-        <f>$F15*Outputs_Internal!M$51/12</f>
+        <f>$F15*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q15" s="67">
-        <f>$F15*Outputs_Internal!N$51/12</f>
+        <f>$F15*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S15" s="67">
@@ -5078,23 +5144,23 @@
         <v>0</v>
       </c>
       <c r="M16" s="67">
-        <f>$F16*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F16*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N16" s="67">
-        <f>$F16*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F16*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O16" s="67">
-        <f>$F16*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F16*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P16" s="67">
-        <f>$F16*Outputs_Internal!M$51/12</f>
+        <f>$F16*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q16" s="67">
-        <f>$F16*Outputs_Internal!N$51/12</f>
+        <f>$F16*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S16" s="67">
@@ -5152,36 +5218,36 @@
         <v>0</v>
       </c>
       <c r="M17" s="67">
-        <f>$F17*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F17*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N17" s="67">
-        <f>$F17*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F17*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O17" s="67">
-        <f>$F17*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F17*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P17" s="67">
-        <f>$F17*Outputs_Internal!M$51/12</f>
+        <f>$F17*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q17" s="67">
-        <f>$F17*Outputs_Internal!N$51/12</f>
+        <f>$F17*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S17" s="67">
         <f t="shared" si="1"/>
-        <v>14400</v>
+        <v>13518.75</v>
       </c>
       <c r="T17" s="67">
         <f t="shared" si="2"/>
-        <v>7650</v>
+        <v>7138.125</v>
       </c>
       <c r="U17" s="67">
         <f t="shared" si="3"/>
-        <v>5190</v>
+        <v>4820.625</v>
       </c>
       <c r="V17" s="67">
         <f t="shared" si="4"/>
@@ -5226,23 +5292,23 @@
         <v>0</v>
       </c>
       <c r="M18" s="67">
-        <f>$F18*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F18*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N18" s="67">
-        <f>$F18*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F18*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O18" s="67">
-        <f>$F18*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F18*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P18" s="67">
-        <f>$F18*Outputs_Internal!M$51/12</f>
+        <f>$F18*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q18" s="67">
-        <f>$F18*Outputs_Internal!N$51/12</f>
+        <f>$F18*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S18" s="67">
@@ -5300,23 +5366,23 @@
         <v>0</v>
       </c>
       <c r="M19" s="67">
-        <f>$F19*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F19*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N19" s="67">
-        <f>$F19*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F19*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O19" s="67">
-        <f>$F19*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F19*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P19" s="67">
-        <f>$F19*Outputs_Internal!M$51/12</f>
+        <f>$F19*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q19" s="67">
-        <f>$F19*Outputs_Internal!N$51/12</f>
+        <f>$F19*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S19" s="67">
@@ -5374,36 +5440,36 @@
         <v>0</v>
       </c>
       <c r="M20" s="67">
-        <f>$F20*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F20*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N20" s="67">
-        <f>$F20*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F20*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O20" s="67">
-        <f>$F20*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F20*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P20" s="67">
-        <f>$F20*Outputs_Internal!M$51/12</f>
+        <f>$F20*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q20" s="67">
-        <f>$F20*Outputs_Internal!N$51/12</f>
+        <f>$F20*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S20" s="67">
         <f t="shared" si="1"/>
-        <v>14400</v>
+        <v>13518.75</v>
       </c>
       <c r="T20" s="67">
         <f t="shared" si="2"/>
-        <v>7650</v>
+        <v>7138.125</v>
       </c>
       <c r="U20" s="67">
         <f t="shared" si="3"/>
-        <v>5190</v>
+        <v>4820.625</v>
       </c>
       <c r="V20" s="67">
         <f t="shared" si="4"/>
@@ -5448,23 +5514,23 @@
         <v>0</v>
       </c>
       <c r="M21" s="67">
-        <f>$F21*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F21*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N21" s="67">
-        <f>$F21*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F21*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O21" s="67">
-        <f>$F21*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F21*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P21" s="67">
-        <f>$F21*Outputs_Internal!M$51/12</f>
+        <f>$F21*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q21" s="67">
-        <f>$F21*Outputs_Internal!N$51/12</f>
+        <f>$F21*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S21" s="67">
@@ -5522,23 +5588,23 @@
         <v>0</v>
       </c>
       <c r="M22" s="67">
-        <f>$F22*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F22*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N22" s="67">
-        <f>$F22*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F22*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O22" s="67">
-        <f>$F22*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F22*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P22" s="67">
-        <f>$F22*Outputs_Internal!M$51/12</f>
+        <f>$F22*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q22" s="67">
-        <f>$F22*Outputs_Internal!N$51/12</f>
+        <f>$F22*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S22" s="67">
@@ -5596,36 +5662,36 @@
         <v>0</v>
       </c>
       <c r="M23" s="67">
-        <f>$F23*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F23*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N23" s="67">
-        <f>$F23*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F23*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O23" s="67">
-        <f>$F23*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F23*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P23" s="67">
-        <f>$F23*Outputs_Internal!M$51/12</f>
+        <f>$F23*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q23" s="67">
-        <f>$F23*Outputs_Internal!N$51/12</f>
+        <f>$F23*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S23" s="67">
         <f t="shared" si="1"/>
-        <v>14400</v>
+        <v>13518.75</v>
       </c>
       <c r="T23" s="67">
         <f t="shared" si="2"/>
-        <v>7650</v>
+        <v>7138.125</v>
       </c>
       <c r="U23" s="67">
         <f t="shared" si="3"/>
-        <v>5190</v>
+        <v>4820.625</v>
       </c>
       <c r="V23" s="67">
         <f t="shared" si="4"/>
@@ -5670,23 +5736,23 @@
         <v>0</v>
       </c>
       <c r="M24" s="67">
-        <f>$F24*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F24*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N24" s="67">
-        <f>$F24*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F24*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O24" s="67">
-        <f>$F24*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F24*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P24" s="67">
-        <f>$F24*Outputs_Internal!M$51/12</f>
+        <f>$F24*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q24" s="67">
-        <f>$F24*Outputs_Internal!N$51/12</f>
+        <f>$F24*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S24" s="67">
@@ -5744,23 +5810,23 @@
         <v>0</v>
       </c>
       <c r="M25" s="67">
-        <f>$F25*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F25*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N25" s="67">
-        <f>$F25*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F25*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O25" s="67">
-        <f>$F25*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F25*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P25" s="67">
-        <f>$F25*Outputs_Internal!M$51/12</f>
+        <f>$F25*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q25" s="67">
-        <f>$F25*Outputs_Internal!N$51/12</f>
+        <f>$F25*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S25" s="67">
@@ -5818,36 +5884,36 @@
         <v>0</v>
       </c>
       <c r="M26" s="67">
-        <f>$F26*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F26*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N26" s="67">
-        <f>$F26*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F26*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O26" s="67">
-        <f>$F26*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F26*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P26" s="67">
-        <f>$F26*Outputs_Internal!M$51/12</f>
+        <f>$F26*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q26" s="67">
-        <f>$F26*Outputs_Internal!N$51/12</f>
+        <f>$F26*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S26" s="67">
         <f t="shared" si="1"/>
-        <v>14400</v>
+        <v>13518.75</v>
       </c>
       <c r="T26" s="67">
         <f t="shared" si="2"/>
-        <v>7650</v>
+        <v>7138.125</v>
       </c>
       <c r="U26" s="67">
         <f t="shared" si="3"/>
-        <v>5190</v>
+        <v>4820.625</v>
       </c>
       <c r="V26" s="67">
         <f t="shared" si="4"/>
@@ -5892,23 +5958,23 @@
         <v>0</v>
       </c>
       <c r="M27" s="67">
-        <f>$F27*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F27*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N27" s="67">
-        <f>$F27*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F27*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O27" s="67">
-        <f>$F27*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F27*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P27" s="67">
-        <f>$F27*Outputs_Internal!M$51/12</f>
+        <f>$F27*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q27" s="67">
-        <f>$F27*Outputs_Internal!N$51/12</f>
+        <f>$F27*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S27" s="67">
@@ -5966,23 +6032,23 @@
         <v>0</v>
       </c>
       <c r="M28" s="67">
-        <f>$F28*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F28*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N28" s="67">
-        <f>$F28*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F28*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O28" s="67">
-        <f>$F28*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F28*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P28" s="67">
-        <f>$F28*Outputs_Internal!M$51/12</f>
+        <f>$F28*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q28" s="67">
-        <f>$F28*Outputs_Internal!N$51/12</f>
+        <f>$F28*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S28" s="67">
@@ -6040,36 +6106,36 @@
         <v>0</v>
       </c>
       <c r="M29" s="67">
-        <f>$F29*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F29*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N29" s="67">
-        <f>$F29*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F29*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O29" s="67">
-        <f>$F29*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F29*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P29" s="67">
-        <f>$F29*Outputs_Internal!M$51/12</f>
+        <f>$F29*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q29" s="67">
-        <f>$F29*Outputs_Internal!N$51/12</f>
+        <f>$F29*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S29" s="67">
         <f t="shared" si="1"/>
-        <v>14400</v>
+        <v>13518.75</v>
       </c>
       <c r="T29" s="67">
         <f t="shared" si="2"/>
-        <v>7650</v>
+        <v>7138.125</v>
       </c>
       <c r="U29" s="67">
         <f t="shared" si="3"/>
-        <v>5190</v>
+        <v>4820.625</v>
       </c>
       <c r="V29" s="67">
         <f t="shared" si="4"/>
@@ -6114,23 +6180,23 @@
         <v>0</v>
       </c>
       <c r="M30" s="67">
-        <f>$F30*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F30*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N30" s="67">
-        <f>$F30*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F30*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O30" s="67">
-        <f>$F30*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F30*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P30" s="67">
-        <f>$F30*Outputs_Internal!M$51/12</f>
+        <f>$F30*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q30" s="67">
-        <f>$F30*Outputs_Internal!N$51/12</f>
+        <f>$F30*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S30" s="67">
@@ -6188,23 +6254,23 @@
         <v>0</v>
       </c>
       <c r="M31" s="67">
-        <f>$F31*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F31*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N31" s="67">
-        <f>$F31*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F31*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O31" s="67">
-        <f>$F31*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F31*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P31" s="67">
-        <f>$F31*Outputs_Internal!M$51/12</f>
+        <f>$F31*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q31" s="67">
-        <f>$F31*Outputs_Internal!N$51/12</f>
+        <f>$F31*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S31" s="67">
@@ -6262,36 +6328,36 @@
         <v>0</v>
       </c>
       <c r="M32" s="67">
-        <f>$F32*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F32*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N32" s="67">
-        <f>$F32*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F32*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O32" s="67">
-        <f>$F32*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F32*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P32" s="67">
-        <f>$F32*Outputs_Internal!M$51/12</f>
+        <f>$F32*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q32" s="67">
-        <f>$F32*Outputs_Internal!N$51/12</f>
+        <f>$F32*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S32" s="67">
         <f t="shared" si="1"/>
-        <v>14400</v>
+        <v>13518.75</v>
       </c>
       <c r="T32" s="67">
         <f t="shared" si="2"/>
-        <v>7650</v>
+        <v>7138.125</v>
       </c>
       <c r="U32" s="67">
         <f t="shared" si="3"/>
-        <v>5190</v>
+        <v>4820.625</v>
       </c>
       <c r="V32" s="67">
         <f t="shared" si="4"/>
@@ -6336,23 +6402,23 @@
         <v>0</v>
       </c>
       <c r="M33" s="67">
-        <f>$F33*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F33*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N33" s="67">
-        <f>$F33*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F33*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O33" s="67">
-        <f>$F33*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F33*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P33" s="67">
-        <f>$F33*Outputs_Internal!M$51/12</f>
+        <f>$F33*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q33" s="67">
-        <f>$F33*Outputs_Internal!N$51/12</f>
+        <f>$F33*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S33" s="67">
@@ -6410,23 +6476,23 @@
         <v>0</v>
       </c>
       <c r="M34" s="67">
-        <f>$F34*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F34*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N34" s="67">
-        <f>$F34*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F34*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O34" s="67">
-        <f>$F34*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F34*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P34" s="67">
-        <f>$F34*Outputs_Internal!M$51/12</f>
+        <f>$F34*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q34" s="67">
-        <f>$F34*Outputs_Internal!N$51/12</f>
+        <f>$F34*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S34" s="67">
@@ -6484,36 +6550,36 @@
         <v>0</v>
       </c>
       <c r="M35" s="67">
-        <f>$F35*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F35*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N35" s="67">
-        <f>$F35*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F35*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O35" s="67">
-        <f>$F35*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F35*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P35" s="67">
-        <f>$F35*Outputs_Internal!M$51/12</f>
+        <f>$F35*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q35" s="67">
-        <f>$F35*Outputs_Internal!N$51/12</f>
+        <f>$F35*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S35" s="67">
         <f t="shared" si="1"/>
-        <v>14400</v>
+        <v>13518.75</v>
       </c>
       <c r="T35" s="67">
         <f t="shared" si="2"/>
-        <v>7650</v>
+        <v>7138.125</v>
       </c>
       <c r="U35" s="67">
         <f t="shared" si="3"/>
-        <v>5190</v>
+        <v>4820.625</v>
       </c>
       <c r="V35" s="67">
         <f t="shared" si="4"/>
@@ -6558,23 +6624,23 @@
         <v>0</v>
       </c>
       <c r="M36" s="67">
-        <f>$F36*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F36*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N36" s="67">
-        <f>$F36*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F36*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O36" s="67">
-        <f>$F36*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F36*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P36" s="67">
-        <f>$F36*Outputs_Internal!M$51/12</f>
+        <f>$F36*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q36" s="67">
-        <f>$F36*Outputs_Internal!N$51/12</f>
+        <f>$F36*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S36" s="67">
@@ -6632,23 +6698,23 @@
         <v>0</v>
       </c>
       <c r="M37" s="67">
-        <f>$F37*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F37*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N37" s="67">
-        <f>$F37*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F37*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O37" s="67">
-        <f>$F37*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F37*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P37" s="67">
-        <f>$F37*Outputs_Internal!M$51/12</f>
+        <f>$F37*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q37" s="67">
-        <f>$F37*Outputs_Internal!N$51/12</f>
+        <f>$F37*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S37" s="67">
@@ -6706,36 +6772,36 @@
         <v>0</v>
       </c>
       <c r="M38" s="67">
-        <f>$F38*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F38*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N38" s="67">
-        <f>$F38*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F38*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O38" s="67">
-        <f>$F38*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F38*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P38" s="67">
-        <f>$F38*Outputs_Internal!M$51/12</f>
+        <f>$F38*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q38" s="67">
-        <f>$F38*Outputs_Internal!N$51/12</f>
+        <f>$F38*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S38" s="67">
         <f t="shared" si="1"/>
-        <v>14400</v>
+        <v>13518.75</v>
       </c>
       <c r="T38" s="67">
         <f t="shared" si="2"/>
-        <v>7650</v>
+        <v>7138.125</v>
       </c>
       <c r="U38" s="67">
         <f t="shared" si="3"/>
-        <v>5190</v>
+        <v>4820.625</v>
       </c>
       <c r="V38" s="67">
         <f t="shared" si="4"/>
@@ -6780,23 +6846,23 @@
         <v>0</v>
       </c>
       <c r="M39" s="67">
-        <f>$F39*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F39*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N39" s="67">
-        <f>$F39*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F39*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O39" s="67">
-        <f>$F39*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F39*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P39" s="67">
-        <f>$F39*Outputs_Internal!M$51/12</f>
+        <f>$F39*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q39" s="67">
-        <f>$F39*Outputs_Internal!N$51/12</f>
+        <f>$F39*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S39" s="67">
@@ -6854,23 +6920,23 @@
         <v>0</v>
       </c>
       <c r="M40" s="67">
-        <f>$F40*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F40*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N40" s="67">
-        <f>$F40*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F40*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O40" s="67">
-        <f>$F40*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F40*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P40" s="67">
-        <f>$F40*Outputs_Internal!M$51/12</f>
+        <f>$F40*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q40" s="67">
-        <f>$F40*Outputs_Internal!N$51/12</f>
+        <f>$F40*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S40" s="67">
@@ -6928,36 +6994,36 @@
         <v>0</v>
       </c>
       <c r="M41" s="67">
-        <f>$F41*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F41*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N41" s="67">
-        <f>$F41*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F41*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O41" s="67">
-        <f>$F41*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F41*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P41" s="67">
-        <f>$F41*Outputs_Internal!M$51/12</f>
+        <f>$F41*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q41" s="67">
-        <f>$F41*Outputs_Internal!N$51/12</f>
+        <f>$F41*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S41" s="67">
         <f t="shared" si="1"/>
-        <v>14400</v>
+        <v>13518.75</v>
       </c>
       <c r="T41" s="67">
         <f t="shared" si="2"/>
-        <v>7650</v>
+        <v>7138.125</v>
       </c>
       <c r="U41" s="67">
         <f t="shared" si="3"/>
-        <v>5190</v>
+        <v>4820.625</v>
       </c>
       <c r="V41" s="67">
         <f t="shared" si="4"/>
@@ -7002,23 +7068,23 @@
         <v>0</v>
       </c>
       <c r="M42" s="67">
-        <f>$F42*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F42*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N42" s="67">
-        <f>$F42*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F42*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O42" s="67">
-        <f>$F42*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F42*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P42" s="67">
-        <f>$F42*Outputs_Internal!M$51/12</f>
+        <f>$F42*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q42" s="67">
-        <f>$F42*Outputs_Internal!N$51/12</f>
+        <f>$F42*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S42" s="67">
@@ -7076,23 +7142,23 @@
         <v>0</v>
       </c>
       <c r="M43" s="67">
-        <f>$F43*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F43*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N43" s="67">
-        <f>$F43*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F43*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O43" s="67">
-        <f>$F43*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F43*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P43" s="67">
-        <f>$F43*Outputs_Internal!M$51/12</f>
+        <f>$F43*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q43" s="67">
-        <f>$F43*Outputs_Internal!N$51/12</f>
+        <f>$F43*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S43" s="67">
@@ -7150,36 +7216,36 @@
         <v>0</v>
       </c>
       <c r="M44" s="67">
-        <f>$F44*Outputs_Internal!$D$51/12</f>
-        <v>4800</v>
+        <f>$F44*Outputs_Internal!$D$52/12</f>
+        <v>4506.25</v>
       </c>
       <c r="N44" s="67">
-        <f>$F44*Outputs_Internal!K$51/12</f>
-        <v>2550</v>
+        <f>$F44*Outputs_Internal!K$52/12</f>
+        <v>2379.375</v>
       </c>
       <c r="O44" s="67">
-        <f>$F44*Outputs_Internal!L$51/12</f>
-        <v>1730</v>
+        <f>$F44*Outputs_Internal!L$52/12</f>
+        <v>1606.875</v>
       </c>
       <c r="P44" s="67">
-        <f>$F44*Outputs_Internal!M$51/12</f>
+        <f>$F44*Outputs_Internal!M$52/12</f>
         <v>480</v>
       </c>
       <c r="Q44" s="67">
-        <f>$F44*Outputs_Internal!N$51/12</f>
+        <f>$F44*Outputs_Internal!N$52/12</f>
         <v>40</v>
       </c>
       <c r="S44" s="67">
         <f>IF(MOD(MONTH($B44),3)=0,SUM(H42:H44,M42:M44),0)</f>
-        <v>14400</v>
+        <v>13518.75</v>
       </c>
       <c r="T44" s="67">
         <f t="shared" si="2"/>
-        <v>7650</v>
+        <v>7138.125</v>
       </c>
       <c r="U44" s="67">
         <f t="shared" si="3"/>
-        <v>5190</v>
+        <v>4820.625</v>
       </c>
       <c r="V44" s="67">
         <f t="shared" si="4"/>
@@ -7224,23 +7290,23 @@
         <v>0</v>
       </c>
       <c r="M45" s="67">
-        <f>$F45*Outputs_Internal!$D$51/12</f>
+        <f>$F45*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N45" s="67">
-        <f>$F45*Outputs_Internal!K$51/12</f>
+        <f>$F45*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O45" s="67">
-        <f>$F45*Outputs_Internal!L$51/12</f>
+        <f>$F45*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P45" s="67">
-        <f>$F45*Outputs_Internal!M$51/12</f>
+        <f>$F45*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q45" s="67">
-        <f>$F45*Outputs_Internal!N$51/12</f>
+        <f>$F45*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S45" s="67">
@@ -7298,23 +7364,23 @@
         <v>0</v>
       </c>
       <c r="M46" s="67">
-        <f>$F46*Outputs_Internal!$D$51/12</f>
+        <f>$F46*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N46" s="67">
-        <f>$F46*Outputs_Internal!K$51/12</f>
+        <f>$F46*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O46" s="67">
-        <f>$F46*Outputs_Internal!L$51/12</f>
+        <f>$F46*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P46" s="67">
-        <f>$F46*Outputs_Internal!M$51/12</f>
+        <f>$F46*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q46" s="67">
-        <f>$F46*Outputs_Internal!N$51/12</f>
+        <f>$F46*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S46" s="67">
@@ -7372,23 +7438,23 @@
         <v>0</v>
       </c>
       <c r="M47" s="67">
-        <f>$F47*Outputs_Internal!$D$51/12</f>
+        <f>$F47*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N47" s="67">
-        <f>$F47*Outputs_Internal!K$51/12</f>
+        <f>$F47*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O47" s="67">
-        <f>$F47*Outputs_Internal!L$51/12</f>
+        <f>$F47*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P47" s="67">
-        <f>$F47*Outputs_Internal!M$51/12</f>
+        <f>$F47*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q47" s="67">
-        <f>$F47*Outputs_Internal!N$51/12</f>
+        <f>$F47*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S47" s="67">
@@ -7446,23 +7512,23 @@
         <v>0</v>
       </c>
       <c r="M48" s="67">
-        <f>$F48*Outputs_Internal!$D$51/12</f>
+        <f>$F48*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N48" s="67">
-        <f>$F48*Outputs_Internal!K$51/12</f>
+        <f>$F48*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O48" s="67">
-        <f>$F48*Outputs_Internal!L$51/12</f>
+        <f>$F48*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P48" s="67">
-        <f>$F48*Outputs_Internal!M$51/12</f>
+        <f>$F48*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q48" s="67">
-        <f>$F48*Outputs_Internal!N$51/12</f>
+        <f>$F48*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S48" s="67">
@@ -7520,23 +7586,23 @@
         <v>0</v>
       </c>
       <c r="M49" s="67">
-        <f>$F49*Outputs_Internal!$D$51/12</f>
+        <f>$F49*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N49" s="67">
-        <f>$F49*Outputs_Internal!K$51/12</f>
+        <f>$F49*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O49" s="67">
-        <f>$F49*Outputs_Internal!L$51/12</f>
+        <f>$F49*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P49" s="67">
-        <f>$F49*Outputs_Internal!M$51/12</f>
+        <f>$F49*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q49" s="67">
-        <f>$F49*Outputs_Internal!N$51/12</f>
+        <f>$F49*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S49" s="67">
@@ -7594,23 +7660,23 @@
         <v>0</v>
       </c>
       <c r="M50" s="67">
-        <f>$F50*Outputs_Internal!$D$51/12</f>
+        <f>$F50*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N50" s="67">
-        <f>$F50*Outputs_Internal!K$51/12</f>
+        <f>$F50*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O50" s="67">
-        <f>$F50*Outputs_Internal!L$51/12</f>
+        <f>$F50*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P50" s="67">
-        <f>$F50*Outputs_Internal!M$51/12</f>
+        <f>$F50*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q50" s="67">
-        <f>$F50*Outputs_Internal!N$51/12</f>
+        <f>$F50*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S50" s="67">
@@ -7668,23 +7734,23 @@
         <v>0</v>
       </c>
       <c r="M51" s="67">
-        <f>$F51*Outputs_Internal!$D$51/12</f>
+        <f>$F51*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N51" s="67">
-        <f>$F51*Outputs_Internal!K$51/12</f>
+        <f>$F51*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O51" s="67">
-        <f>$F51*Outputs_Internal!L$51/12</f>
+        <f>$F51*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P51" s="67">
-        <f>$F51*Outputs_Internal!M$51/12</f>
+        <f>$F51*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q51" s="67">
-        <f>$F51*Outputs_Internal!N$51/12</f>
+        <f>$F51*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S51" s="67">
@@ -7742,23 +7808,23 @@
         <v>0</v>
       </c>
       <c r="M52" s="67">
-        <f>$F52*Outputs_Internal!$D$51/12</f>
+        <f>$F52*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N52" s="67">
-        <f>$F52*Outputs_Internal!K$51/12</f>
+        <f>$F52*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O52" s="67">
-        <f>$F52*Outputs_Internal!L$51/12</f>
+        <f>$F52*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P52" s="67">
-        <f>$F52*Outputs_Internal!M$51/12</f>
+        <f>$F52*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q52" s="67">
-        <f>$F52*Outputs_Internal!N$51/12</f>
+        <f>$F52*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S52" s="67">
@@ -7816,23 +7882,23 @@
         <v>0</v>
       </c>
       <c r="M53" s="67">
-        <f>$F53*Outputs_Internal!$D$51/12</f>
+        <f>$F53*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N53" s="67">
-        <f>$F53*Outputs_Internal!K$51/12</f>
+        <f>$F53*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O53" s="67">
-        <f>$F53*Outputs_Internal!L$51/12</f>
+        <f>$F53*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P53" s="67">
-        <f>$F53*Outputs_Internal!M$51/12</f>
+        <f>$F53*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q53" s="67">
-        <f>$F53*Outputs_Internal!N$51/12</f>
+        <f>$F53*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S53" s="67">
@@ -7890,23 +7956,23 @@
         <v>0</v>
       </c>
       <c r="M54" s="67">
-        <f>$F54*Outputs_Internal!$D$51/12</f>
+        <f>$F54*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N54" s="67">
-        <f>$F54*Outputs_Internal!K$51/12</f>
+        <f>$F54*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O54" s="67">
-        <f>$F54*Outputs_Internal!L$51/12</f>
+        <f>$F54*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P54" s="67">
-        <f>$F54*Outputs_Internal!M$51/12</f>
+        <f>$F54*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q54" s="67">
-        <f>$F54*Outputs_Internal!N$51/12</f>
+        <f>$F54*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S54" s="67">
@@ -7964,23 +8030,23 @@
         <v>0</v>
       </c>
       <c r="M55" s="67">
-        <f>$F55*Outputs_Internal!$D$51/12</f>
+        <f>$F55*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N55" s="67">
-        <f>$F55*Outputs_Internal!K$51/12</f>
+        <f>$F55*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O55" s="67">
-        <f>$F55*Outputs_Internal!L$51/12</f>
+        <f>$F55*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P55" s="67">
-        <f>$F55*Outputs_Internal!M$51/12</f>
+        <f>$F55*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q55" s="67">
-        <f>$F55*Outputs_Internal!N$51/12</f>
+        <f>$F55*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S55" s="67">
@@ -8038,23 +8104,23 @@
         <v>0</v>
       </c>
       <c r="M56" s="67">
-        <f>$F56*Outputs_Internal!$D$51/12</f>
+        <f>$F56*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N56" s="67">
-        <f>$F56*Outputs_Internal!K$51/12</f>
+        <f>$F56*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O56" s="67">
-        <f>$F56*Outputs_Internal!L$51/12</f>
+        <f>$F56*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P56" s="67">
-        <f>$F56*Outputs_Internal!M$51/12</f>
+        <f>$F56*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q56" s="67">
-        <f>$F56*Outputs_Internal!N$51/12</f>
+        <f>$F56*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S56" s="67">
@@ -8112,23 +8178,23 @@
         <v>0</v>
       </c>
       <c r="M57" s="67">
-        <f>$F57*Outputs_Internal!$D$51/12</f>
+        <f>$F57*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N57" s="67">
-        <f>$F57*Outputs_Internal!K$51/12</f>
+        <f>$F57*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O57" s="67">
-        <f>$F57*Outputs_Internal!L$51/12</f>
+        <f>$F57*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P57" s="67">
-        <f>$F57*Outputs_Internal!M$51/12</f>
+        <f>$F57*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q57" s="67">
-        <f>$F57*Outputs_Internal!N$51/12</f>
+        <f>$F57*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S57" s="67">
@@ -8186,23 +8252,23 @@
         <v>0</v>
       </c>
       <c r="M58" s="67">
-        <f>$F58*Outputs_Internal!$D$51/12</f>
+        <f>$F58*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N58" s="67">
-        <f>$F58*Outputs_Internal!K$51/12</f>
+        <f>$F58*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O58" s="67">
-        <f>$F58*Outputs_Internal!L$51/12</f>
+        <f>$F58*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P58" s="67">
-        <f>$F58*Outputs_Internal!M$51/12</f>
+        <f>$F58*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q58" s="67">
-        <f>$F58*Outputs_Internal!N$51/12</f>
+        <f>$F58*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S58" s="67">
@@ -8260,23 +8326,23 @@
         <v>0</v>
       </c>
       <c r="M59" s="67">
-        <f>$F59*Outputs_Internal!$D$51/12</f>
+        <f>$F59*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N59" s="67">
-        <f>$F59*Outputs_Internal!K$51/12</f>
+        <f>$F59*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O59" s="67">
-        <f>$F59*Outputs_Internal!L$51/12</f>
+        <f>$F59*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P59" s="67">
-        <f>$F59*Outputs_Internal!M$51/12</f>
+        <f>$F59*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q59" s="67">
-        <f>$F59*Outputs_Internal!N$51/12</f>
+        <f>$F59*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S59" s="67">
@@ -8334,23 +8400,23 @@
         <v>0</v>
       </c>
       <c r="M60" s="67">
-        <f>$F60*Outputs_Internal!$D$51/12</f>
+        <f>$F60*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N60" s="67">
-        <f>$F60*Outputs_Internal!K$51/12</f>
+        <f>$F60*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O60" s="67">
-        <f>$F60*Outputs_Internal!L$51/12</f>
+        <f>$F60*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P60" s="67">
-        <f>$F60*Outputs_Internal!M$51/12</f>
+        <f>$F60*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q60" s="67">
-        <f>$F60*Outputs_Internal!N$51/12</f>
+        <f>$F60*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S60" s="67">
@@ -8408,23 +8474,23 @@
         <v>0</v>
       </c>
       <c r="M61" s="67">
-        <f>$F61*Outputs_Internal!$D$51/12</f>
+        <f>$F61*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N61" s="67">
-        <f>$F61*Outputs_Internal!K$51/12</f>
+        <f>$F61*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O61" s="67">
-        <f>$F61*Outputs_Internal!L$51/12</f>
+        <f>$F61*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P61" s="67">
-        <f>$F61*Outputs_Internal!M$51/12</f>
+        <f>$F61*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q61" s="67">
-        <f>$F61*Outputs_Internal!N$51/12</f>
+        <f>$F61*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S61" s="67">
@@ -8482,23 +8548,23 @@
         <v>0</v>
       </c>
       <c r="M62" s="67">
-        <f>$F62*Outputs_Internal!$D$51/12</f>
+        <f>$F62*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N62" s="67">
-        <f>$F62*Outputs_Internal!K$51/12</f>
+        <f>$F62*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O62" s="67">
-        <f>$F62*Outputs_Internal!L$51/12</f>
+        <f>$F62*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P62" s="67">
-        <f>$F62*Outputs_Internal!M$51/12</f>
+        <f>$F62*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q62" s="67">
-        <f>$F62*Outputs_Internal!N$51/12</f>
+        <f>$F62*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S62" s="67">
@@ -8556,23 +8622,23 @@
         <v>0</v>
       </c>
       <c r="M63" s="67">
-        <f>$F63*Outputs_Internal!$D$51/12</f>
+        <f>$F63*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N63" s="67">
-        <f>$F63*Outputs_Internal!K$51/12</f>
+        <f>$F63*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O63" s="67">
-        <f>$F63*Outputs_Internal!L$51/12</f>
+        <f>$F63*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P63" s="67">
-        <f>$F63*Outputs_Internal!M$51/12</f>
+        <f>$F63*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q63" s="67">
-        <f>$F63*Outputs_Internal!N$51/12</f>
+        <f>$F63*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S63" s="67">
@@ -8630,23 +8696,23 @@
         <v>0</v>
       </c>
       <c r="M64" s="67">
-        <f>$F64*Outputs_Internal!$D$51/12</f>
+        <f>$F64*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N64" s="67">
-        <f>$F64*Outputs_Internal!K$51/12</f>
+        <f>$F64*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O64" s="67">
-        <f>$F64*Outputs_Internal!L$51/12</f>
+        <f>$F64*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P64" s="67">
-        <f>$F64*Outputs_Internal!M$51/12</f>
+        <f>$F64*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q64" s="67">
-        <f>$F64*Outputs_Internal!N$51/12</f>
+        <f>$F64*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S64" s="67">
@@ -8704,23 +8770,23 @@
         <v>0</v>
       </c>
       <c r="M65" s="67">
-        <f>$F65*Outputs_Internal!$D$51/12</f>
+        <f>$F65*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N65" s="67">
-        <f>$F65*Outputs_Internal!K$51/12</f>
+        <f>$F65*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O65" s="67">
-        <f>$F65*Outputs_Internal!L$51/12</f>
+        <f>$F65*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P65" s="67">
-        <f>$F65*Outputs_Internal!M$51/12</f>
+        <f>$F65*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q65" s="67">
-        <f>$F65*Outputs_Internal!N$51/12</f>
+        <f>$F65*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S65" s="67">
@@ -8778,23 +8844,23 @@
         <v>0</v>
       </c>
       <c r="M66" s="67">
-        <f>$F66*Outputs_Internal!$D$51/12</f>
+        <f>$F66*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N66" s="67">
-        <f>$F66*Outputs_Internal!K$51/12</f>
+        <f>$F66*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O66" s="67">
-        <f>$F66*Outputs_Internal!L$51/12</f>
+        <f>$F66*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P66" s="67">
-        <f>$F66*Outputs_Internal!M$51/12</f>
+        <f>$F66*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q66" s="67">
-        <f>$F66*Outputs_Internal!N$51/12</f>
+        <f>$F66*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S66" s="67">
@@ -8852,23 +8918,23 @@
         <v>0</v>
       </c>
       <c r="M67" s="67">
-        <f>$F67*Outputs_Internal!$D$51/12</f>
+        <f>$F67*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N67" s="67">
-        <f>$F67*Outputs_Internal!K$51/12</f>
+        <f>$F67*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O67" s="67">
-        <f>$F67*Outputs_Internal!L$51/12</f>
+        <f>$F67*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P67" s="67">
-        <f>$F67*Outputs_Internal!M$51/12</f>
+        <f>$F67*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q67" s="67">
-        <f>$F67*Outputs_Internal!N$51/12</f>
+        <f>$F67*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S67" s="67">
@@ -8926,23 +8992,23 @@
         <v>0</v>
       </c>
       <c r="M68" s="67">
-        <f>$F68*Outputs_Internal!$D$51/12</f>
+        <f>$F68*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N68" s="67">
-        <f>$F68*Outputs_Internal!K$51/12</f>
+        <f>$F68*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O68" s="67">
-        <f>$F68*Outputs_Internal!L$51/12</f>
+        <f>$F68*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P68" s="67">
-        <f>$F68*Outputs_Internal!M$51/12</f>
+        <f>$F68*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q68" s="67">
-        <f>$F68*Outputs_Internal!N$51/12</f>
+        <f>$F68*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S68" s="67">
@@ -9000,23 +9066,23 @@
         <v>0</v>
       </c>
       <c r="M69" s="67">
-        <f>$F69*Outputs_Internal!$D$51/12</f>
+        <f>$F69*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N69" s="67">
-        <f>$F69*Outputs_Internal!K$51/12</f>
+        <f>$F69*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O69" s="67">
-        <f>$F69*Outputs_Internal!L$51/12</f>
+        <f>$F69*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P69" s="67">
-        <f>$F69*Outputs_Internal!M$51/12</f>
+        <f>$F69*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q69" s="67">
-        <f>$F69*Outputs_Internal!N$51/12</f>
+        <f>$F69*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S69" s="67">
@@ -9074,23 +9140,23 @@
         <v>0</v>
       </c>
       <c r="M70" s="67">
-        <f>$F70*Outputs_Internal!$D$51/12</f>
+        <f>$F70*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N70" s="67">
-        <f>$F70*Outputs_Internal!K$51/12</f>
+        <f>$F70*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O70" s="67">
-        <f>$F70*Outputs_Internal!L$51/12</f>
+        <f>$F70*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P70" s="67">
-        <f>$F70*Outputs_Internal!M$51/12</f>
+        <f>$F70*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q70" s="67">
-        <f>$F70*Outputs_Internal!N$51/12</f>
+        <f>$F70*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S70" s="67">
@@ -9148,23 +9214,23 @@
         <v>0</v>
       </c>
       <c r="M71" s="67">
-        <f>$F71*Outputs_Internal!$D$51/12</f>
+        <f>$F71*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N71" s="67">
-        <f>$F71*Outputs_Internal!K$51/12</f>
+        <f>$F71*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O71" s="67">
-        <f>$F71*Outputs_Internal!L$51/12</f>
+        <f>$F71*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P71" s="67">
-        <f>$F71*Outputs_Internal!M$51/12</f>
+        <f>$F71*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q71" s="67">
-        <f>$F71*Outputs_Internal!N$51/12</f>
+        <f>$F71*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S71" s="67">
@@ -9222,23 +9288,23 @@
         <v>0</v>
       </c>
       <c r="M72" s="67">
-        <f>$F72*Outputs_Internal!$D$51/12</f>
+        <f>$F72*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N72" s="67">
-        <f>$F72*Outputs_Internal!K$51/12</f>
+        <f>$F72*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O72" s="67">
-        <f>$F72*Outputs_Internal!L$51/12</f>
+        <f>$F72*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P72" s="67">
-        <f>$F72*Outputs_Internal!M$51/12</f>
+        <f>$F72*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q72" s="67">
-        <f>$F72*Outputs_Internal!N$51/12</f>
+        <f>$F72*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S72" s="67">
@@ -9296,23 +9362,23 @@
         <v>0</v>
       </c>
       <c r="M73" s="67">
-        <f>$F73*Outputs_Internal!$D$51/12</f>
+        <f>$F73*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N73" s="67">
-        <f>$F73*Outputs_Internal!K$51/12</f>
+        <f>$F73*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O73" s="67">
-        <f>$F73*Outputs_Internal!L$51/12</f>
+        <f>$F73*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P73" s="67">
-        <f>$F73*Outputs_Internal!M$51/12</f>
+        <f>$F73*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q73" s="67">
-        <f>$F73*Outputs_Internal!N$51/12</f>
+        <f>$F73*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S73" s="67">
@@ -9370,23 +9436,23 @@
         <v>0</v>
       </c>
       <c r="M74" s="67">
-        <f>$F74*Outputs_Internal!$D$51/12</f>
+        <f>$F74*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N74" s="67">
-        <f>$F74*Outputs_Internal!K$51/12</f>
+        <f>$F74*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O74" s="67">
-        <f>$F74*Outputs_Internal!L$51/12</f>
+        <f>$F74*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P74" s="67">
-        <f>$F74*Outputs_Internal!M$51/12</f>
+        <f>$F74*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q74" s="67">
-        <f>$F74*Outputs_Internal!N$51/12</f>
+        <f>$F74*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S74" s="67">
@@ -9444,23 +9510,23 @@
         <v>0</v>
       </c>
       <c r="M75" s="67">
-        <f>$F75*Outputs_Internal!$D$51/12</f>
+        <f>$F75*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N75" s="67">
-        <f>$F75*Outputs_Internal!K$51/12</f>
+        <f>$F75*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O75" s="67">
-        <f>$F75*Outputs_Internal!L$51/12</f>
+        <f>$F75*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P75" s="67">
-        <f>$F75*Outputs_Internal!M$51/12</f>
+        <f>$F75*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q75" s="67">
-        <f>$F75*Outputs_Internal!N$51/12</f>
+        <f>$F75*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S75" s="67">
@@ -9518,23 +9584,23 @@
         <v>0</v>
       </c>
       <c r="M76" s="67">
-        <f>$F76*Outputs_Internal!$D$51/12</f>
+        <f>$F76*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N76" s="67">
-        <f>$F76*Outputs_Internal!K$51/12</f>
+        <f>$F76*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O76" s="67">
-        <f>$F76*Outputs_Internal!L$51/12</f>
+        <f>$F76*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P76" s="67">
-        <f>$F76*Outputs_Internal!M$51/12</f>
+        <f>$F76*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q76" s="67">
-        <f>$F76*Outputs_Internal!N$51/12</f>
+        <f>$F76*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S76" s="67">
@@ -9592,23 +9658,23 @@
         <v>0</v>
       </c>
       <c r="M77" s="67">
-        <f>$F77*Outputs_Internal!$D$51/12</f>
+        <f>$F77*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N77" s="67">
-        <f>$F77*Outputs_Internal!K$51/12</f>
+        <f>$F77*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O77" s="67">
-        <f>$F77*Outputs_Internal!L$51/12</f>
+        <f>$F77*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P77" s="67">
-        <f>$F77*Outputs_Internal!M$51/12</f>
+        <f>$F77*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q77" s="67">
-        <f>$F77*Outputs_Internal!N$51/12</f>
+        <f>$F77*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S77" s="67">
@@ -9666,23 +9732,23 @@
         <v>0</v>
       </c>
       <c r="M78" s="67">
-        <f>$F78*Outputs_Internal!$D$51/12</f>
+        <f>$F78*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N78" s="67">
-        <f>$F78*Outputs_Internal!K$51/12</f>
+        <f>$F78*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O78" s="67">
-        <f>$F78*Outputs_Internal!L$51/12</f>
+        <f>$F78*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P78" s="67">
-        <f>$F78*Outputs_Internal!M$51/12</f>
+        <f>$F78*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q78" s="67">
-        <f>$F78*Outputs_Internal!N$51/12</f>
+        <f>$F78*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S78" s="67">
@@ -9740,23 +9806,23 @@
         <v>0</v>
       </c>
       <c r="M79" s="67">
-        <f>$F79*Outputs_Internal!$D$51/12</f>
+        <f>$F79*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N79" s="67">
-        <f>$F79*Outputs_Internal!K$51/12</f>
+        <f>$F79*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O79" s="67">
-        <f>$F79*Outputs_Internal!L$51/12</f>
+        <f>$F79*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P79" s="67">
-        <f>$F79*Outputs_Internal!M$51/12</f>
+        <f>$F79*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q79" s="67">
-        <f>$F79*Outputs_Internal!N$51/12</f>
+        <f>$F79*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S79" s="67">
@@ -9814,23 +9880,23 @@
         <v>0</v>
       </c>
       <c r="M80" s="67">
-        <f>$F80*Outputs_Internal!$D$51/12</f>
+        <f>$F80*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N80" s="67">
-        <f>$F80*Outputs_Internal!K$51/12</f>
+        <f>$F80*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O80" s="67">
-        <f>$F80*Outputs_Internal!L$51/12</f>
+        <f>$F80*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P80" s="67">
-        <f>$F80*Outputs_Internal!M$51/12</f>
+        <f>$F80*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q80" s="67">
-        <f>$F80*Outputs_Internal!N$51/12</f>
+        <f>$F80*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S80" s="67">
@@ -9888,23 +9954,23 @@
         <v>0</v>
       </c>
       <c r="M81" s="67">
-        <f>$F81*Outputs_Internal!$D$51/12</f>
+        <f>$F81*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N81" s="67">
-        <f>$F81*Outputs_Internal!K$51/12</f>
+        <f>$F81*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O81" s="67">
-        <f>$F81*Outputs_Internal!L$51/12</f>
+        <f>$F81*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P81" s="67">
-        <f>$F81*Outputs_Internal!M$51/12</f>
+        <f>$F81*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q81" s="67">
-        <f>$F81*Outputs_Internal!N$51/12</f>
+        <f>$F81*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S81" s="67">
@@ -9962,23 +10028,23 @@
         <v>0</v>
       </c>
       <c r="M82" s="67">
-        <f>$F82*Outputs_Internal!$D$51/12</f>
+        <f>$F82*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N82" s="67">
-        <f>$F82*Outputs_Internal!K$51/12</f>
+        <f>$F82*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O82" s="67">
-        <f>$F82*Outputs_Internal!L$51/12</f>
+        <f>$F82*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P82" s="67">
-        <f>$F82*Outputs_Internal!M$51/12</f>
+        <f>$F82*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q82" s="67">
-        <f>$F82*Outputs_Internal!N$51/12</f>
+        <f>$F82*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S82" s="67">
@@ -10036,23 +10102,23 @@
         <v>0</v>
       </c>
       <c r="M83" s="67">
-        <f>$F83*Outputs_Internal!$D$51/12</f>
+        <f>$F83*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N83" s="67">
-        <f>$F83*Outputs_Internal!K$51/12</f>
+        <f>$F83*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O83" s="67">
-        <f>$F83*Outputs_Internal!L$51/12</f>
+        <f>$F83*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P83" s="67">
-        <f>$F83*Outputs_Internal!M$51/12</f>
+        <f>$F83*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q83" s="67">
-        <f>$F83*Outputs_Internal!N$51/12</f>
+        <f>$F83*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S83" s="67">
@@ -10110,23 +10176,23 @@
         <v>0</v>
       </c>
       <c r="M84" s="67">
-        <f>$F84*Outputs_Internal!$D$51/12</f>
+        <f>$F84*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N84" s="67">
-        <f>$F84*Outputs_Internal!K$51/12</f>
+        <f>$F84*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O84" s="67">
-        <f>$F84*Outputs_Internal!L$51/12</f>
+        <f>$F84*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P84" s="67">
-        <f>$F84*Outputs_Internal!M$51/12</f>
+        <f>$F84*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q84" s="67">
-        <f>$F84*Outputs_Internal!N$51/12</f>
+        <f>$F84*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S84" s="67">
@@ -10184,23 +10250,23 @@
         <v>0</v>
       </c>
       <c r="M85" s="67">
-        <f>$F85*Outputs_Internal!$D$51/12</f>
+        <f>$F85*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N85" s="67">
-        <f>$F85*Outputs_Internal!K$51/12</f>
+        <f>$F85*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O85" s="67">
-        <f>$F85*Outputs_Internal!L$51/12</f>
+        <f>$F85*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P85" s="67">
-        <f>$F85*Outputs_Internal!M$51/12</f>
+        <f>$F85*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q85" s="67">
-        <f>$F85*Outputs_Internal!N$51/12</f>
+        <f>$F85*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S85" s="67">
@@ -10258,23 +10324,23 @@
         <v>0</v>
       </c>
       <c r="M86" s="67">
-        <f>$F86*Outputs_Internal!$D$51/12</f>
+        <f>$F86*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N86" s="67">
-        <f>$F86*Outputs_Internal!K$51/12</f>
+        <f>$F86*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O86" s="67">
-        <f>$F86*Outputs_Internal!L$51/12</f>
+        <f>$F86*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P86" s="67">
-        <f>$F86*Outputs_Internal!M$51/12</f>
+        <f>$F86*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q86" s="67">
-        <f>$F86*Outputs_Internal!N$51/12</f>
+        <f>$F86*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S86" s="67">
@@ -10332,23 +10398,23 @@
         <v>0</v>
       </c>
       <c r="M87" s="67">
-        <f>$F87*Outputs_Internal!$D$51/12</f>
+        <f>$F87*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N87" s="67">
-        <f>$F87*Outputs_Internal!K$51/12</f>
+        <f>$F87*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O87" s="67">
-        <f>$F87*Outputs_Internal!L$51/12</f>
+        <f>$F87*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P87" s="67">
-        <f>$F87*Outputs_Internal!M$51/12</f>
+        <f>$F87*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q87" s="67">
-        <f>$F87*Outputs_Internal!N$51/12</f>
+        <f>$F87*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S87" s="67">
@@ -10406,23 +10472,23 @@
         <v>0</v>
       </c>
       <c r="M88" s="67">
-        <f>$F88*Outputs_Internal!$D$51/12</f>
+        <f>$F88*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N88" s="67">
-        <f>$F88*Outputs_Internal!K$51/12</f>
+        <f>$F88*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O88" s="67">
-        <f>$F88*Outputs_Internal!L$51/12</f>
+        <f>$F88*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P88" s="67">
-        <f>$F88*Outputs_Internal!M$51/12</f>
+        <f>$F88*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q88" s="67">
-        <f>$F88*Outputs_Internal!N$51/12</f>
+        <f>$F88*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S88" s="67">
@@ -10480,23 +10546,23 @@
         <v>0</v>
       </c>
       <c r="M89" s="67">
-        <f>$F89*Outputs_Internal!$D$51/12</f>
+        <f>$F89*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N89" s="67">
-        <f>$F89*Outputs_Internal!K$51/12</f>
+        <f>$F89*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O89" s="67">
-        <f>$F89*Outputs_Internal!L$51/12</f>
+        <f>$F89*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P89" s="67">
-        <f>$F89*Outputs_Internal!M$51/12</f>
+        <f>$F89*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q89" s="67">
-        <f>$F89*Outputs_Internal!N$51/12</f>
+        <f>$F89*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S89" s="67">
@@ -10554,23 +10620,23 @@
         <v>0</v>
       </c>
       <c r="M90" s="67">
-        <f>$F90*Outputs_Internal!$D$51/12</f>
+        <f>$F90*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N90" s="67">
-        <f>$F90*Outputs_Internal!K$51/12</f>
+        <f>$F90*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O90" s="67">
-        <f>$F90*Outputs_Internal!L$51/12</f>
+        <f>$F90*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P90" s="67">
-        <f>$F90*Outputs_Internal!M$51/12</f>
+        <f>$F90*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q90" s="67">
-        <f>$F90*Outputs_Internal!N$51/12</f>
+        <f>$F90*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S90" s="67">
@@ -10628,23 +10694,23 @@
         <v>0</v>
       </c>
       <c r="M91" s="67">
-        <f>$F91*Outputs_Internal!$D$51/12</f>
+        <f>$F91*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N91" s="67">
-        <f>$F91*Outputs_Internal!K$51/12</f>
+        <f>$F91*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O91" s="67">
-        <f>$F91*Outputs_Internal!L$51/12</f>
+        <f>$F91*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P91" s="67">
-        <f>$F91*Outputs_Internal!M$51/12</f>
+        <f>$F91*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q91" s="67">
-        <f>$F91*Outputs_Internal!N$51/12</f>
+        <f>$F91*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S91" s="67">
@@ -10702,23 +10768,23 @@
         <v>0</v>
       </c>
       <c r="M92" s="67">
-        <f>$F92*Outputs_Internal!$D$51/12</f>
+        <f>$F92*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N92" s="67">
-        <f>$F92*Outputs_Internal!K$51/12</f>
+        <f>$F92*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O92" s="67">
-        <f>$F92*Outputs_Internal!L$51/12</f>
+        <f>$F92*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P92" s="67">
-        <f>$F92*Outputs_Internal!M$51/12</f>
+        <f>$F92*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q92" s="67">
-        <f>$F92*Outputs_Internal!N$51/12</f>
+        <f>$F92*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S92" s="67">
@@ -10776,23 +10842,23 @@
         <v>0</v>
       </c>
       <c r="M93" s="67">
-        <f>$F93*Outputs_Internal!$D$51/12</f>
+        <f>$F93*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N93" s="67">
-        <f>$F93*Outputs_Internal!K$51/12</f>
+        <f>$F93*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O93" s="67">
-        <f>$F93*Outputs_Internal!L$51/12</f>
+        <f>$F93*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P93" s="67">
-        <f>$F93*Outputs_Internal!M$51/12</f>
+        <f>$F93*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q93" s="67">
-        <f>$F93*Outputs_Internal!N$51/12</f>
+        <f>$F93*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S93" s="67">
@@ -10850,23 +10916,23 @@
         <v>0</v>
       </c>
       <c r="M94" s="67">
-        <f>$F94*Outputs_Internal!$D$51/12</f>
+        <f>$F94*Outputs_Internal!$D$52/12</f>
         <v>0</v>
       </c>
       <c r="N94" s="67">
-        <f>$F94*Outputs_Internal!K$51/12</f>
+        <f>$F94*Outputs_Internal!K$52/12</f>
         <v>0</v>
       </c>
       <c r="O94" s="67">
-        <f>$F94*Outputs_Internal!L$51/12</f>
+        <f>$F94*Outputs_Internal!L$52/12</f>
         <v>0</v>
       </c>
       <c r="P94" s="67">
-        <f>$F94*Outputs_Internal!M$51/12</f>
+        <f>$F94*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q94" s="67">
-        <f>$F94*Outputs_Internal!N$51/12</f>
+        <f>$F94*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S94" s="67">
@@ -10902,13 +10968,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O108"/>
+  <dimension ref="B2:O110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D63" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12753,11 +12819,11 @@
         <v>64</v>
       </c>
       <c r="D90" s="1">
-        <f>IF(D98=1, 0, IF(D98=2, $E$101, IF(D98=3, $E$102, IF(D98=4, $E$103, IF(D98=5, $E$104, "")))))</f>
+        <f>IF(D100=1, 0, IF(D100=2, $E$103, IF(D100=3, $E$104, IF(D100=4, $E$105, IF(D100=5, $E$106, "")))))</f>
         <v>0</v>
       </c>
       <c r="E90" s="1">
-        <f t="shared" ref="E90:H90" si="21">IF(E98=1, 0, IF(E98=2, $E$101, IF(E98=3, $E$102, IF(E98=4, $E$103, IF(E98=5, $E$104, "")))))</f>
+        <f t="shared" ref="E90:H90" si="21">IF(E100=1, 0, IF(E100=2, $E$103, IF(E100=3, $E$104, IF(E100=4, $E$105, IF(E100=5, $E$106, "")))))</f>
         <v>0</v>
       </c>
       <c r="F90" s="1">
@@ -12773,172 +12839,200 @@
         <v>0</v>
       </c>
     </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+    </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B92" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D92" s="1">
+        <f>IF(Inputs!$D$4 = "Y", Prices!$I$18, 0)*-1</f>
+        <v>-3525</v>
+      </c>
+      <c r="E92" s="1">
+        <v>0</v>
+      </c>
+      <c r="F92" s="1">
+        <v>0</v>
+      </c>
+      <c r="G92" s="1">
+        <v>0</v>
+      </c>
+      <c r="H92" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B94" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D92" s="7">
+      <c r="D94" s="7">
         <f>SUM(D88, D90)</f>
         <v>57600</v>
       </c>
-      <c r="E92" s="7">
+      <c r="E94" s="7">
         <f>SUM(E88, E90)</f>
         <v>0</v>
       </c>
-      <c r="F92" s="7">
+      <c r="F94" s="7">
         <f>SUM(F88, F90)</f>
         <v>0</v>
       </c>
-      <c r="G92" s="7">
+      <c r="G94" s="7">
         <f>SUM(G88, G90)</f>
         <v>0</v>
       </c>
-      <c r="H92" s="7">
+      <c r="H94" s="7">
         <f>SUM(H88, H90)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="27"/>
-      <c r="C95" s="21" t="s">
+    <row r="97" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B97" s="27"/>
+      <c r="C97" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="D95" s="21">
+      <c r="D97" s="21">
         <f>IFERROR(_xlfn.RANK.EQ(D88,$D$88:$H$88),5)</f>
         <v>1</v>
       </c>
-      <c r="E95" s="21">
-        <f t="shared" ref="E95:H95" si="22">IFERROR(_xlfn.RANK.EQ(E88,$D$88:$H$88),5)</f>
+      <c r="E97" s="21">
+        <f t="shared" ref="E97:H97" si="22">IFERROR(_xlfn.RANK.EQ(E88,$D$88:$H$88),5)</f>
         <v>2</v>
       </c>
-      <c r="F95" s="21">
+      <c r="F97" s="21">
         <f t="shared" si="22"/>
         <v>2</v>
       </c>
-      <c r="G95" s="21">
+      <c r="G97" s="21">
         <f t="shared" si="22"/>
         <v>2</v>
       </c>
-      <c r="H95" s="21">
+      <c r="H97" s="21">
         <f t="shared" si="22"/>
         <v>2</v>
-      </c>
-    </row>
-    <row r="96" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="27"/>
-      <c r="D96" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="E96" s="21">
-        <v>0.2</v>
-      </c>
-      <c r="F96" s="21">
-        <v>0.3</v>
-      </c>
-      <c r="G96" s="21">
-        <v>0.4</v>
-      </c>
-      <c r="H96" s="21">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="97" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="27"/>
-      <c r="D97" s="21">
-        <f>SUM(D95:D96)</f>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E97" s="21">
-        <f t="shared" ref="E97:H97" si="23">SUM(E95:E96)</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F97" s="21">
-        <f t="shared" si="23"/>
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="G97" s="21">
-        <f t="shared" si="23"/>
-        <v>2.4</v>
-      </c>
-      <c r="H97" s="21">
-        <f t="shared" si="23"/>
-        <v>2.5</v>
       </c>
     </row>
     <row r="98" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B98" s="27"/>
       <c r="D98" s="21">
-        <f>_xlfn.RANK.EQ(D97, $D$97:$H$97, 5)</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E98" s="21">
-        <f t="shared" ref="E98:H98" si="24">_xlfn.RANK.EQ(E97, $D$97:$H$97, 5)</f>
+        <v>0.2</v>
+      </c>
+      <c r="F98" s="21">
+        <v>0.3</v>
+      </c>
+      <c r="G98" s="21">
+        <v>0.4</v>
+      </c>
+      <c r="H98" s="21">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="99" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="27"/>
+      <c r="D99" s="21">
+        <f>SUM(D97:D98)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E99" s="21">
+        <f t="shared" ref="E99:H99" si="23">SUM(E97:E98)</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F99" s="21">
+        <f t="shared" si="23"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G99" s="21">
+        <f t="shared" si="23"/>
+        <v>2.4</v>
+      </c>
+      <c r="H99" s="21">
+        <f t="shared" si="23"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="100" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="27"/>
+      <c r="D100" s="21">
+        <f>_xlfn.RANK.EQ(D99, $D$99:$H$99, 5)</f>
+        <v>1</v>
+      </c>
+      <c r="E100" s="21">
+        <f t="shared" ref="E100:H100" si="24">_xlfn.RANK.EQ(E99, $D$99:$H$99, 5)</f>
         <v>2</v>
       </c>
-      <c r="F98" s="21">
+      <c r="F100" s="21">
         <f t="shared" si="24"/>
         <v>3</v>
       </c>
-      <c r="G98" s="21">
+      <c r="G100" s="21">
         <f t="shared" si="24"/>
         <v>4</v>
       </c>
-      <c r="H98" s="21">
+      <c r="H100" s="21">
         <f t="shared" si="24"/>
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="27"/>
-    </row>
-    <row r="100" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="27"/>
-      <c r="C100" s="21" t="s">
-        <v>53</v>
-      </c>
-    </row>
     <row r="101" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B101" s="27"/>
-      <c r="D101" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="E101" s="23">
-        <f>INDEX($D$88:$H$88, 1, MATCH(2, $D$98:$H$98, 0))*Prices!$I$10*-1</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="102" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B102" s="27"/>
-      <c r="D102" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="E102" s="23">
-        <f>INDEX($D$88:$H$88, 1, MATCH(3, $D$98:$H$98, 0))*Prices!$I$11*-1</f>
-        <v>0</v>
+      <c r="C102" s="21" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="103" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B103" s="27"/>
       <c r="D103" s="21" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E103" s="23">
-        <f>INDEX($D$88:$H$88, 1, MATCH(4, $D$98:$H$98, 0))*Prices!$I$11*-1</f>
+        <f>INDEX($D$88:$H$88, 1, MATCH(2, $D$100:$H$100, 0))*Prices!$I$10*-1</f>
         <v>0</v>
       </c>
     </row>
     <row r="104" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B104" s="27"/>
       <c r="D104" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E104" s="23">
+        <f>INDEX($D$88:$H$88, 1, MATCH(3, $D$100:$H$100, 0))*Prices!$I$11*-1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B105" s="27"/>
+      <c r="D105" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E105" s="23">
+        <f>INDEX($D$88:$H$88, 1, MATCH(4, $D$100:$H$100, 0))*Prices!$I$11*-1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B106" s="27"/>
+      <c r="D106" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="E104" s="23">
-        <f>INDEX($D$88:$H$88, 1, MATCH(5, $D$98:$H$98, 0))*Prices!$I$11*-1</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F108" s="2"/>
+      <c r="E106" s="23">
+        <f>INDEX($D$88:$H$88, 1, MATCH(5, $D$100:$H$100, 0))*Prices!$I$11*-1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F110" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12950,7 +13044,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13175,7 +13271,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="19" t="s">
         <v>15</v>
       </c>
@@ -13186,7 +13282,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="19" t="s">
         <v>34</v>
       </c>
@@ -13196,12 +13292,18 @@
       <c r="D18" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="H18" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="I18" s="2">
+        <v>3525</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C19" s="44"/>
       <c r="D19" s="40"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="17" t="s">
         <v>17</v>
       </c>
@@ -13212,7 +13314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="17" t="s">
         <v>18</v>
       </c>
@@ -13223,7 +13325,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="19" t="s">
         <v>19</v>
       </c>
@@ -13234,7 +13336,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="19" t="s">
         <v>20</v>
       </c>
@@ -13247,5 +13349,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>